<commit_message>
Implemented version 1.1 of the VCM SOP
</commit_message>
<xml_diff>
--- a/docs/cc_data_generator.xlsx
+++ b/docs/cc_data_generator.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>OPTION_NAME</t>
   </si>
@@ -121,6 +121,15 @@
   </si>
   <si>
     <t>The test APEX server hostname</t>
+  </si>
+  <si>
+    <t>DLM_SYSTEM_STATUS</t>
+  </si>
+  <si>
+    <t>PROD</t>
+  </si>
+  <si>
+    <t>Database Logging Module data system status - this configuration option determines which messages are logged in the database</t>
   </si>
 </sst>
 </file>
@@ -438,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,6 +652,21 @@
         <v>INSERT INTO CC_CONFIG_OPTIONS (OPTION_NAME, OPTION_VALUE, OPTION_DESC) VALUES ('TEST_HOSTNAME', 'picmidt.nmfs.local', 'The test APEX server hostname');</v>
       </c>
     </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" t="str">
+        <f>"INSERT INTO CC_CONFIG_OPTIONS ("&amp;$A$1&amp;", "&amp;$B$1&amp;", "&amp;$C$1&amp;") VALUES ('"&amp;SUBSTITUTE(A14, "'", "''")&amp;"', '"&amp;SUBSTITUTE(B14, "'", "''")&amp;"', '"&amp;SUBSTITUTE(C14, "'", "''")&amp;"');"</f>
+        <v>INSERT INTO CC_CONFIG_OPTIONS (OPTION_NAME, OPTION_VALUE, OPTION_DESC) VALUES ('DLM_SYSTEM_STATUS', 'PROD', 'Database Logging Module data system status - this configuration option determines which messages are logged in the database');</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>